<commit_message>
- update component sheet - add vumeter pcb fo 32 and 66 Hz (number calculated based on resistor values)
</commit_message>
<xml_diff>
--- a/03_Others/freq_comp_list.xlsx
+++ b/03_Others/freq_comp_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitProjects\9_Nixie_IN-13\03_Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61BFCF93-983F-451B-9612-6A7AA5D4FE54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7566A49-CF2C-4CDB-A304-F77BEBA98F38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="3465" windowWidth="19365" windowHeight="11160" xr2:uid="{8A845EE5-4A4A-4CF9-A8C0-AFDC8359B486}"/>
+    <workbookView xWindow="16500" yWindow="1080" windowWidth="19365" windowHeight="11160" xr2:uid="{8A845EE5-4A4A-4CF9-A8C0-AFDC8359B486}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,136 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Andrei Holingher</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{2C96D930-A9FF-4E3B-86DA-D58A37F0AE42}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andrei Holingher:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+15k + 10k</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{6F767D48-34F7-436E-BEFC-8ACA575EEC0C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andrei Holingher:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+10k || 10k</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{C575B609-91B3-4C2D-922C-7293AF223AE2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andrei Holingher:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+10k + 2k</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{6DEE0B40-6ED8-40BE-9159-95C685214CF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andrei Holingher:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+2.2k + 200</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{57898008-BA94-4CBB-86FB-F9A8359E04C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Andrei Holingher:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+10k + 2.2k</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
@@ -189,7 +319,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +340,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -554,11 +697,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B515ADE-3078-4E26-9831-77C82E2C6689}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B515ADE-3078-4E26-9831-77C82E2C6689}">
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +709,7 @@
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -811,5 +954,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remake less wires, strong connections
</commit_message>
<xml_diff>
--- a/03_Others/freq_comp_list.xlsx
+++ b/03_Others/freq_comp_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitProjects\9_Nixie_IN-13\03_Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7566A49-CF2C-4CDB-A304-F77BEBA98F38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CE2316-948A-475F-8A84-E3579B2EF094}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="1080" windowWidth="19365" windowHeight="11160" xr2:uid="{8A845EE5-4A4A-4CF9-A8C0-AFDC8359B486}"/>
+    <workbookView xWindow="0" yWindow="3780" windowWidth="23040" windowHeight="12204" xr2:uid="{8A845EE5-4A4A-4CF9-A8C0-AFDC8359B486}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-15k + 10k</t>
+19k + 5k</t>
         </r>
       </text>
     </comment>
@@ -355,12 +355,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -375,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,6 +390,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,18 +710,18 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -735,8 +744,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -755,8 +764,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -778,7 +787,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -801,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -821,8 +830,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -841,8 +850,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -864,7 +873,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -887,7 +896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -907,8 +916,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -927,8 +936,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">

</xml_diff>